<commit_message>
Updated the date field: 5/12/19
</commit_message>
<xml_diff>
--- a/Basketball Stats.xlsx
+++ b/Basketball Stats.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\Desktop\Basketball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\BasketballTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA883AE-5370-4D5B-AE6B-72637D65B52C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1DA2ADD-0204-4301-B8D3-BDC71C2E667E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Basketball Data" sheetId="1" r:id="rId1"/>
     <sheet name="March Madness" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,22 +577,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F713E613-1833-4B50-9741-1975199B9C96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="H303" sqref="H303"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -627,7 +626,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>IF(MOD(ROW(A2)-1,8)=0,A2+1,A2)</f>
         <v>1</v>
@@ -646,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">IF(MOD(ROW(A3)-1,8)=0,A3+1,A3)</f>
         <v>1</v>
@@ -665,7 +664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -684,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -703,7 +702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -722,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -741,7 +740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -760,7 +759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -780,7 +779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -800,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -820,7 +819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -840,7 +839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -860,7 +859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -880,7 +879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -900,7 +899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -920,7 +919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -940,7 +939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -960,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -980,7 +979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1000,7 +999,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1020,7 +1019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1040,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1060,7 +1059,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1080,7 +1079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1100,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1120,7 +1119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1140,7 +1139,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1160,7 +1159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1180,7 +1179,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1200,7 +1199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1220,7 +1219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1240,7 +1239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1259,7 +1258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1279,7 +1278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1299,7 +1298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1319,7 +1318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1339,7 +1338,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1359,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1379,7 +1378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1399,7 +1398,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1419,7 +1418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1439,7 +1438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1459,7 +1458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1479,7 +1478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1499,7 +1498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1519,7 +1518,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1539,7 +1538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1559,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1579,7 +1578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1599,7 +1598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1619,7 +1618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1639,7 +1638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1659,7 +1658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1679,7 +1678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1699,7 +1698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1719,7 +1718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1739,7 +1738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1759,7 +1758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1779,7 +1778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1799,7 +1798,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1819,7 +1818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1839,7 +1838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1859,7 +1858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1879,7 +1878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1898,7 +1897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1918,7 +1917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" ref="A68:A132" si="4">IF(MOD(ROW(A67)-1,8)=0,A67+1,A67)</f>
         <v>9</v>
@@ -1938,7 +1937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1958,7 +1957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1978,7 +1977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1998,7 +1997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -2018,7 +2017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -2038,7 +2037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2058,7 +2057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2078,7 +2077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2098,7 +2097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2118,7 +2117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2138,7 +2137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2158,7 +2157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2178,7 +2177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2198,7 +2197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2218,7 +2217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2238,7 +2237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2258,7 +2257,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2278,7 +2277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2298,7 +2297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2318,7 +2317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2338,7 +2337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2358,7 +2357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2378,7 +2377,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2398,7 +2397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2418,7 +2417,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2438,7 +2437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2458,7 +2457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2478,7 +2477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2498,7 +2497,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2518,7 +2517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2537,7 +2536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2557,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2577,7 +2576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2597,7 +2596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2617,7 +2616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2637,7 +2636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2657,7 +2656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2677,7 +2676,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2697,7 +2696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2717,7 +2716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2737,7 +2736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2757,7 +2756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2777,7 +2776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2797,7 +2796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2817,7 +2816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2837,7 +2836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2857,7 +2856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2877,7 +2876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2897,7 +2896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2917,7 +2916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2937,7 +2936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2957,7 +2956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2977,7 +2976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2997,7 +2996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3017,7 +3016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3037,7 +3036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3057,7 +3056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3077,7 +3076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3097,7 +3096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3117,7 +3116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3137,7 +3136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3157,7 +3156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -3177,7 +3176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -3197,7 +3196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -3217,7 +3216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <f t="shared" ref="A133:A196" si="8">IF(MOD(ROW(A132)-1,8)=0,A132+1,A132)</f>
         <v>17</v>
@@ -3237,7 +3236,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3257,7 +3256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3277,7 +3276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3297,7 +3296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3317,7 +3316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3336,7 +3335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3356,7 +3355,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3376,7 +3375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3396,7 +3395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3416,7 +3415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3436,7 +3435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3456,7 +3455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3476,7 +3475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3496,7 +3495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3516,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3536,7 +3535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3556,7 +3555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3576,7 +3575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3596,7 +3595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3616,7 +3615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3636,7 +3635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3656,7 +3655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3676,7 +3675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3696,7 +3695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3716,7 +3715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3736,7 +3735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3756,7 +3755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3776,7 +3775,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3796,7 +3795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3816,7 +3815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3836,7 +3835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3856,7 +3855,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3876,7 +3875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3896,7 +3895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3916,7 +3915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3936,7 +3935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3956,7 +3955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -3975,7 +3974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -3995,7 +3994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4015,7 +4014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4035,7 +4034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4055,7 +4054,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4075,7 +4074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4095,7 +4094,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4115,7 +4114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4135,7 +4134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4155,7 +4154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4175,7 +4174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4195,7 +4194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4215,7 +4214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4235,7 +4234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4255,7 +4254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4275,7 +4274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4295,7 +4294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4315,7 +4314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4335,7 +4334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4355,7 +4354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4375,7 +4374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4395,7 +4394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4415,7 +4414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4435,7 +4434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -4454,7 +4453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -4474,7 +4473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -4494,7 +4493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <f t="shared" ref="A197:A260" si="11">IF(MOD(ROW(A196)-1,8)=0,A196+1,A196)</f>
         <v>25</v>
@@ -4514,7 +4513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4534,7 +4533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4554,7 +4553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4574,7 +4573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4594,7 +4593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4614,7 +4613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4634,7 +4633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4654,7 +4653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4674,7 +4673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4694,7 +4693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4714,7 +4713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4734,7 +4733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4754,7 +4753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4774,7 +4773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4794,7 +4793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4814,7 +4813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4834,7 +4833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4854,7 +4853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4874,7 +4873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4894,7 +4893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4914,7 +4913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4934,7 +4933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4954,7 +4953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4974,7 +4973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4994,7 +4993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5014,7 +5013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5034,7 +5033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5054,7 +5053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5074,7 +5073,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5094,7 +5093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5114,7 +5113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5134,7 +5133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5154,7 +5153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5174,7 +5173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5194,7 +5193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5214,7 +5213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5234,7 +5233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5253,7 +5252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5273,7 +5272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5293,7 +5292,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5313,7 +5312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5333,7 +5332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5353,7 +5352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5373,7 +5372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5393,7 +5392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5413,7 +5412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5433,7 +5432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5453,7 +5452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5473,7 +5472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5493,7 +5492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5513,7 +5512,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5533,7 +5532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5553,7 +5552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5573,7 +5572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5593,7 +5592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5613,7 +5612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5633,7 +5632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5653,7 +5652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5673,7 +5672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5693,7 +5692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5713,7 +5712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -5732,7 +5731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -5752,7 +5751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -5772,7 +5771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <f t="shared" ref="A261:A313" si="15">IF(MOD(ROW(A260)-1,8)=0,A260+1,A260)</f>
         <v>33</v>
@@ -5792,7 +5791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5812,7 +5811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5832,7 +5831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5852,7 +5851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5872,7 +5871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5892,7 +5891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5912,7 +5911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5932,7 +5931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5952,7 +5951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5972,7 +5971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5992,7 +5991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -6012,7 +6011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -6032,7 +6031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6052,7 +6051,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6072,7 +6071,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6092,7 +6091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6112,7 +6111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6132,7 +6131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6152,7 +6151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6172,7 +6171,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6192,7 +6191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6212,7 +6211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6232,7 +6231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6252,7 +6251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6272,7 +6271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6292,7 +6291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6312,7 +6311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6332,7 +6331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6352,17 +6351,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
-      <c r="B290" s="6">
-        <f t="shared" ref="B290:B312" si="16">IF(A290="","",B289)</f>
-        <v>43589</v>
+      <c r="B290" s="5">
+        <v>43597</v>
       </c>
       <c r="C290" t="str">
-        <f t="shared" ref="C290:C312" si="17">IF(A290="","",C282)</f>
+        <f t="shared" ref="C290:C312" si="16">IF(A290="","",C282)</f>
         <v>RoBert</v>
       </c>
       <c r="D290" s="2">
@@ -6372,17 +6370,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B291" s="6">
+        <f t="shared" ref="B290:B312" si="17">IF(A291="","",B290)</f>
+        <v>43597</v>
+      </c>
+      <c r="C291" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C291" t="str">
-        <f t="shared" si="17"/>
         <v>Alex</v>
       </c>
       <c r="D291" s="2">
@@ -6392,17 +6390,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B292" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C292" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C292" t="str">
-        <f t="shared" si="17"/>
         <v>Evan</v>
       </c>
       <c r="D292" s="2">
@@ -6412,17 +6410,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B293" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C293" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C293" t="str">
-        <f t="shared" si="17"/>
         <v>Andy</v>
       </c>
       <c r="D293" s="2">
@@ -6432,17 +6430,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B294" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C294" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C294" t="str">
-        <f t="shared" si="17"/>
         <v>Phil</v>
       </c>
       <c r="D294" s="2">
@@ -6452,17 +6450,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B295" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C295" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C295" t="str">
-        <f t="shared" si="17"/>
         <v>Ben</v>
       </c>
       <c r="D295" s="2">
@@ -6472,17 +6470,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B296" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C296" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C296" t="str">
-        <f t="shared" si="17"/>
         <v>Jeff</v>
       </c>
       <c r="D296" s="2">
@@ -6492,17 +6490,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B297" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C297" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C297" t="str">
-        <f t="shared" si="17"/>
         <v>Tim</v>
       </c>
       <c r="D297" s="2">
@@ -6512,17 +6510,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B298" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C298" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C298" t="str">
-        <f t="shared" si="17"/>
         <v>RoBert</v>
       </c>
       <c r="D298" s="2">
@@ -6532,17 +6530,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B299" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C299" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C299" t="str">
-        <f t="shared" si="17"/>
         <v>Alex</v>
       </c>
       <c r="D299" s="2">
@@ -6552,17 +6550,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B300" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C300" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C300" t="str">
-        <f t="shared" si="17"/>
         <v>Evan</v>
       </c>
       <c r="D300" s="2">
@@ -6572,17 +6570,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B301" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C301" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C301" t="str">
-        <f t="shared" si="17"/>
         <v>Andy</v>
       </c>
       <c r="D301" s="2">
@@ -6592,17 +6590,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B302" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C302" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C302" t="str">
-        <f t="shared" si="17"/>
         <v>Phil</v>
       </c>
       <c r="D302" s="2">
@@ -6612,17 +6610,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B303" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C303" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C303" t="str">
-        <f t="shared" si="17"/>
         <v>Ben</v>
       </c>
       <c r="D303" s="2">
@@ -6632,17 +6630,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B304" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C304" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C304" t="str">
-        <f t="shared" si="17"/>
         <v>Jeff</v>
       </c>
       <c r="D304" s="2">
@@ -6652,17 +6650,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
       </c>
       <c r="B305" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C305" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C305" t="str">
-        <f t="shared" si="17"/>
         <v>Tim</v>
       </c>
       <c r="D305" s="2">
@@ -6672,17 +6670,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B306" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C306" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C306" t="str">
-        <f t="shared" si="17"/>
         <v>RoBert</v>
       </c>
       <c r="D306" s="2">
@@ -6692,17 +6690,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B307" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C307" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C307" t="str">
-        <f t="shared" si="17"/>
         <v>Alex</v>
       </c>
       <c r="D307" s="2">
@@ -6712,17 +6710,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B308" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C308" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C308" t="str">
-        <f t="shared" si="17"/>
         <v>Evan</v>
       </c>
       <c r="D308" s="2">
@@ -6732,17 +6730,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B309" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C309" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C309" t="str">
-        <f t="shared" si="17"/>
         <v>Andy</v>
       </c>
       <c r="D309" s="2">
@@ -6752,17 +6750,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B310" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C310" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C310" t="str">
-        <f t="shared" si="17"/>
         <v>Phil</v>
       </c>
       <c r="D310" s="2">
@@ -6772,17 +6770,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B311" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C311" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C311" t="str">
-        <f t="shared" si="17"/>
         <v>Ben</v>
       </c>
       <c r="D311" s="2">
@@ -6792,17 +6790,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B312" s="6">
+        <f t="shared" si="17"/>
+        <v>43597</v>
+      </c>
+      <c r="C312" t="str">
         <f t="shared" si="16"/>
-        <v>43589</v>
-      </c>
-      <c r="C312" t="str">
-        <f t="shared" si="17"/>
         <v>Jeff</v>
       </c>
       <c r="D312" s="2">
@@ -6812,14 +6810,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B313" s="6">
         <f t="shared" ref="B313" si="18">IF(A313="","",B312)</f>
-        <v>43589</v>
+        <v>43597</v>
       </c>
       <c r="C313" t="str">
         <f t="shared" ref="C313" si="19">IF(A313="","",C305)</f>
@@ -6832,751 +6830,751 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="6"/>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="6"/>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="6"/>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="6"/>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="6"/>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="6"/>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="6"/>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="6"/>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="6"/>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="6"/>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="6"/>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="6"/>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="6"/>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="6"/>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="6"/>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="6"/>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="6"/>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="6"/>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="6"/>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="6"/>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="6"/>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="6"/>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="6"/>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="6"/>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="6"/>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="6"/>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="6"/>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="6"/>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="6"/>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="6"/>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="6"/>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="6"/>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="6"/>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="6"/>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="6"/>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="6"/>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="6"/>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1"/>
       <c r="B351" s="6"/>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1"/>
       <c r="B352" s="6"/>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1"/>
       <c r="B353" s="6"/>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1"/>
       <c r="B354" s="6"/>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
       <c r="B355" s="6"/>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
       <c r="B356" s="6"/>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="6"/>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="6"/>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="6"/>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
       <c r="B360" s="6"/>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1"/>
       <c r="B361" s="6"/>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1"/>
       <c r="B362" s="6"/>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1"/>
       <c r="B363" s="6"/>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1"/>
       <c r="B364" s="6"/>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="1"/>
       <c r="B365" s="6"/>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="1"/>
       <c r="B366" s="6"/>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
       <c r="B367" s="6"/>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
       <c r="B368" s="6"/>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="1"/>
       <c r="B369" s="6"/>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
       <c r="B370" s="6"/>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
       <c r="B371" s="6"/>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
       <c r="B372" s="6"/>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
       <c r="B373" s="6"/>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
       <c r="B374" s="6"/>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
       <c r="B375" s="6"/>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
       <c r="B376" s="6"/>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
       <c r="B377" s="6"/>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
       <c r="B378" s="6"/>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
       <c r="B379" s="6"/>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
       <c r="B380" s="6"/>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
       <c r="B381" s="6"/>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1"/>
       <c r="B382" s="6"/>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1"/>
       <c r="B383" s="6"/>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="1"/>
       <c r="B384" s="6"/>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="1"/>
       <c r="B385" s="6"/>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1"/>
       <c r="B386" s="6"/>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1"/>
       <c r="B387" s="6"/>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1"/>
       <c r="B388" s="6"/>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1"/>
       <c r="B389" s="6"/>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="1"/>
       <c r="B390" s="6"/>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="1"/>
       <c r="B391" s="6"/>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1"/>
       <c r="B392" s="6"/>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="1"/>
       <c r="B393" s="6"/>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1"/>
       <c r="B394" s="6"/>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1"/>
       <c r="B395" s="6"/>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1"/>
       <c r="B396" s="6"/>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="1"/>
       <c r="B397" s="6"/>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="1"/>
       <c r="B398" s="6"/>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1"/>
       <c r="B399" s="6"/>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="1"/>
       <c r="B400" s="6"/>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1"/>
       <c r="B401" s="6"/>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="1"/>
       <c r="B402" s="6"/>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1"/>
       <c r="B403" s="6"/>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="1"/>
       <c r="B404" s="6"/>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="1"/>
       <c r="B405" s="6"/>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="1"/>
       <c r="B406" s="6"/>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="1"/>
       <c r="B407" s="6"/>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="1"/>
       <c r="B408" s="6"/>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="1"/>
       <c r="B409" s="6"/>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="1"/>
       <c r="B410" s="6"/>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="1"/>
       <c r="B411" s="6"/>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1"/>
       <c r="B412" s="6"/>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1"/>
       <c r="B413" s="6"/>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1"/>
       <c r="B414" s="6"/>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="1"/>
       <c r="B415" s="6"/>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="1"/>
       <c r="B416" s="6"/>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="1"/>
       <c r="B417" s="6"/>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="1"/>
       <c r="B418" s="6"/>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="1"/>
       <c r="B419" s="6"/>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="1"/>
       <c r="B420" s="6"/>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="1"/>
       <c r="B421" s="6"/>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="1"/>
       <c r="B422" s="6"/>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="1"/>
       <c r="B423" s="6"/>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="1"/>
       <c r="B424" s="6"/>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="1"/>
       <c r="B425" s="6"/>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="1"/>
       <c r="B426" s="6"/>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="1"/>
       <c r="B427" s="6"/>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="1"/>
       <c r="B428" s="6"/>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="1"/>
       <c r="B429" s="6"/>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="1"/>
       <c r="B430" s="6"/>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="1"/>
       <c r="B431" s="6"/>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="1"/>
       <c r="B432" s="6"/>
     </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="1"/>
       <c r="B433" s="6"/>
     </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="1"/>
       <c r="B434" s="6"/>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="1"/>
       <c r="B435" s="6"/>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="1"/>
       <c r="B436" s="6"/>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="1"/>
       <c r="B437" s="6"/>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="1"/>
       <c r="B438" s="6"/>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="1"/>
       <c r="B439" s="6"/>
     </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="1"/>
       <c r="B440" s="6"/>
     </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="1"/>
       <c r="B441" s="6"/>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="1"/>
       <c r="B442" s="6"/>
     </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="1"/>
       <c r="B443" s="6"/>
     </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="1"/>
       <c r="B444" s="6"/>
     </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="1"/>
       <c r="B445" s="6"/>
     </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" s="1"/>
       <c r="B446" s="6"/>
     </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" s="1"/>
       <c r="B447" s="6"/>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="1"/>
       <c r="B448" s="6"/>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" s="1"/>
       <c r="B449" s="6"/>
     </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" s="1"/>
       <c r="B450" s="6"/>
     </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" s="1"/>
       <c r="B451" s="6"/>
     </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" s="1"/>
       <c r="B452" s="6"/>
     </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" s="1"/>
       <c r="B453" s="6"/>
     </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" s="1"/>
       <c r="B454" s="6"/>
     </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" s="1"/>
       <c r="B455" s="6"/>
     </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" s="1"/>
       <c r="B456" s="6"/>
     </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" s="1"/>
       <c r="B457" s="6"/>
     </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="1"/>
       <c r="B458" s="6"/>
     </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" s="1"/>
       <c r="B459" s="6"/>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" s="1"/>
       <c r="B460" s="6"/>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" s="1"/>
       <c r="B461" s="6"/>
     </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" s="1"/>
       <c r="B462" s="6"/>
     </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" s="1"/>
       <c r="B463" s="6"/>
     </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="1"/>
       <c r="B464" s="6"/>
     </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" s="1"/>
       <c r="B465" s="6"/>
     </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" s="1"/>
       <c r="B466" s="6"/>
     </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" s="1"/>
       <c r="B467" s="6"/>
     </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" s="1"/>
       <c r="B468" s="6"/>
     </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" s="1"/>
       <c r="B469" s="6"/>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" s="1"/>
       <c r="B470" s="6"/>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" s="1"/>
       <c r="B471" s="6"/>
     </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" s="1"/>
       <c r="B472" s="6"/>
     </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" s="1"/>
       <c r="B473" s="6"/>
     </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" s="1"/>
       <c r="B474" s="6"/>
     </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" s="1"/>
       <c r="B475" s="6"/>
     </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" s="1"/>
       <c r="B476" s="6"/>
     </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" s="1"/>
       <c r="B477" s="6"/>
     </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" s="1"/>
       <c r="B478" s="6"/>
     </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" s="1"/>
       <c r="B479" s="6"/>
     </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" s="1"/>
       <c r="B480" s="6"/>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" s="1"/>
       <c r="B481" s="6"/>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" s="1"/>
       <c r="B482" s="6"/>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A483" s="1"/>
       <c r="B483" s="6"/>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A484" s="1"/>
       <c r="B484" s="6"/>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" s="1"/>
       <c r="B485" s="6"/>
     </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A486" s="1"/>
       <c r="B486" s="6"/>
     </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A487" s="1"/>
       <c r="B487" s="6"/>
     </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A488" s="1"/>
       <c r="B488" s="6"/>
     </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A489" s="1"/>
       <c r="B489" s="6"/>
     </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A490" s="1"/>
       <c r="B490" s="6"/>
     </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A491" s="1"/>
       <c r="B491" s="6"/>
     </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A492" s="1"/>
       <c r="B492" s="6"/>
     </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A493" s="1"/>
       <c r="B493" s="6"/>
     </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A494" s="1"/>
       <c r="B494" s="6"/>
     </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A495" s="1"/>
       <c r="B495" s="6"/>
     </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" s="1"/>
       <c r="B496" s="6"/>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A497" s="1"/>
       <c r="B497" s="6"/>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A498" s="1"/>
       <c r="B498" s="6"/>
     </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A499" s="1"/>
       <c r="B499" s="6"/>
     </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A500" s="1"/>
       <c r="B500" s="6"/>
     </row>
@@ -7587,27 +7585,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642C60B7-2249-4268-A61E-EBE7E329571F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -7669,7 +7667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>2019</v>
       </c>
@@ -7738,7 +7736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" ref="A3:A9" si="0">A2</f>
         <v>2019</v>
@@ -7808,7 +7806,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7876,7 +7874,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7946,7 +7944,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8016,7 +8014,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8086,7 +8084,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8156,7 +8154,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>

</xml_diff>

<commit_message>
Added in August 25th data
</commit_message>
<xml_diff>
--- a/Basketball Stats.xlsx
+++ b/Basketball Stats.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\BasketballTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\Desktop\Basketball\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6D0C7-3B45-41F2-9588-8F6E3B5BA744}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basketball Data" sheetId="1" r:id="rId1"/>
     <sheet name="March Madness" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -171,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,22 +578,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="B290" sqref="B290"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -626,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>IF(MOD(ROW(A2)-1,8)=0,A2+1,A2)</f>
         <v>1</v>
@@ -645,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="0">IF(MOD(ROW(A3)-1,8)=0,A3+1,A3)</f>
         <v>1</v>
@@ -664,7 +665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -683,7 +684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -702,7 +703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -721,7 +722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -740,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -759,7 +760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -779,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -799,7 +800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -819,7 +820,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -839,7 +840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -859,7 +860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -879,7 +880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -899,7 +900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -919,7 +920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -939,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -959,7 +960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -979,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -999,7 +1000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1019,7 +1020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1039,7 +1040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1059,7 +1060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1079,7 +1080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1099,7 +1100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1119,7 +1120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1139,7 +1140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1159,7 +1160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1179,7 +1180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1199,7 +1200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1219,7 +1220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1239,7 +1240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1258,7 +1259,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1278,7 +1279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1298,7 +1299,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1318,7 +1319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1338,7 +1339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1358,7 +1359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1378,7 +1379,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1398,7 +1399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1418,7 +1419,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1438,7 +1439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1458,7 +1459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1478,7 +1479,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1498,7 +1499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1518,7 +1519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1538,7 +1539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1558,7 +1559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1578,7 +1579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1598,7 +1599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1618,7 +1619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1638,7 +1639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1658,7 +1659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1678,7 +1679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1698,7 +1699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1718,7 +1719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1738,7 +1739,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1758,7 +1759,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1778,7 +1779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1798,7 +1799,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1818,7 +1819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1838,7 +1839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1858,7 +1859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1878,7 +1879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1897,7 +1898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1917,7 +1918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <f t="shared" ref="A68:A132" si="4">IF(MOD(ROW(A67)-1,8)=0,A67+1,A67)</f>
         <v>9</v>
@@ -1937,7 +1938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1957,7 +1958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1977,7 +1978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -1997,7 +1998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -2017,7 +2018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -2037,7 +2038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2057,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2077,7 +2078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2097,7 +2098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2117,7 +2118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2137,7 +2138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2157,7 +2158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2177,7 +2178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2197,7 +2198,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2217,7 +2218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2237,7 +2238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2257,7 +2258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2277,7 +2278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2297,7 +2298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2317,7 +2318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2337,7 +2338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2357,7 +2358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2377,7 +2378,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2397,7 +2398,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2417,7 +2418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2437,7 +2438,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2457,7 +2458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2477,7 +2478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2497,7 +2498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2517,7 +2518,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2536,7 +2537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2556,7 +2557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2576,7 +2577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2596,7 +2597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2616,7 +2617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2636,7 +2637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2656,7 +2657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2676,7 +2677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2696,7 +2697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2716,7 +2717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2736,7 +2737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2756,7 +2757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2776,7 +2777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2796,7 +2797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2816,7 +2817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2836,7 +2837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2856,7 +2857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2876,7 +2877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2896,7 +2897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2916,7 +2917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2936,7 +2937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2956,7 +2957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2976,7 +2977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2996,7 +2997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3016,7 +3017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3036,7 +3037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3056,7 +3057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3076,7 +3077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3096,7 +3097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3116,7 +3117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3136,7 +3137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -3156,7 +3157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -3176,7 +3177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -3196,7 +3197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -3216,7 +3217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <f t="shared" ref="A133:A196" si="8">IF(MOD(ROW(A132)-1,8)=0,A132+1,A132)</f>
         <v>17</v>
@@ -3236,7 +3237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3256,7 +3257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3276,7 +3277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3296,7 +3297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <f t="shared" si="8"/>
         <v>17</v>
@@ -3316,7 +3317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3335,7 +3336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3355,7 +3356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3375,7 +3376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3395,7 +3396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3415,7 +3416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3435,7 +3436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3455,7 +3456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <f t="shared" si="8"/>
         <v>18</v>
@@ -3475,7 +3476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3495,7 +3496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3515,7 +3516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3535,7 +3536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3555,7 +3556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3575,7 +3576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3595,7 +3596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3615,7 +3616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <f t="shared" si="8"/>
         <v>19</v>
@@ -3635,7 +3636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3655,7 +3656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3675,7 +3676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3695,7 +3696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3715,7 +3716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3735,7 +3736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3755,7 +3756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3775,7 +3776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <f t="shared" si="8"/>
         <v>20</v>
@@ -3795,7 +3796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3815,7 +3816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3835,7 +3836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3855,7 +3856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3875,7 +3876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3895,7 +3896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3915,7 +3916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3935,7 +3936,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <f t="shared" si="8"/>
         <v>21</v>
@@ -3955,7 +3956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -3974,7 +3975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -3994,7 +3995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4014,7 +4015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4034,7 +4035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4054,7 +4055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4074,7 +4075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4094,7 +4095,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <f t="shared" si="8"/>
         <v>22</v>
@@ -4114,7 +4115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4134,7 +4135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4154,7 +4155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4174,7 +4175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4194,7 +4195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4214,7 +4215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4234,7 +4235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4254,7 +4255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <f t="shared" si="8"/>
         <v>23</v>
@@ -4274,7 +4275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4294,7 +4295,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4314,7 +4315,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4334,7 +4335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4354,7 +4355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4374,7 +4375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4394,7 +4395,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4414,7 +4415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <f t="shared" si="8"/>
         <v>24</v>
@@ -4434,7 +4435,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -4453,7 +4454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -4473,7 +4474,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <f t="shared" si="8"/>
         <v>25</v>
@@ -4493,7 +4494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <f t="shared" ref="A197:A260" si="11">IF(MOD(ROW(A196)-1,8)=0,A196+1,A196)</f>
         <v>25</v>
@@ -4513,7 +4514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4533,7 +4534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4553,7 +4554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4573,7 +4574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <f t="shared" si="11"/>
         <v>25</v>
@@ -4593,7 +4594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4613,7 +4614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4633,7 +4634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4653,7 +4654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4673,7 +4674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4693,7 +4694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4713,7 +4714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4733,7 +4734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <f t="shared" si="11"/>
         <v>26</v>
@@ -4753,7 +4754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4773,7 +4774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4793,7 +4794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4813,7 +4814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4833,7 +4834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4853,7 +4854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4873,7 +4874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4893,7 +4894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <f t="shared" si="11"/>
         <v>27</v>
@@ -4913,7 +4914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4933,7 +4934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4953,7 +4954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4973,7 +4974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -4993,7 +4994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5013,7 +5014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5033,7 +5034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5053,7 +5054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <f t="shared" si="11"/>
         <v>28</v>
@@ -5073,7 +5074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5093,7 +5094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5113,7 +5114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5133,7 +5134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5153,7 +5154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5173,7 +5174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5193,7 +5194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5213,7 +5214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <f t="shared" si="11"/>
         <v>29</v>
@@ -5233,7 +5234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5252,7 +5253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5272,7 +5273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5292,7 +5293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5312,7 +5313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5332,7 +5333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5352,7 +5353,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5372,7 +5373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <f t="shared" si="11"/>
         <v>30</v>
@@ -5392,7 +5393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5412,7 +5413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5432,7 +5433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5452,7 +5453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5472,7 +5473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5492,7 +5493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5512,7 +5513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5532,7 +5533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <f t="shared" si="11"/>
         <v>31</v>
@@ -5552,7 +5553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5572,7 +5573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5592,7 +5593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5612,7 +5613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5632,7 +5633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5652,7 +5653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5672,7 +5673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5692,7 +5693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <f t="shared" si="11"/>
         <v>32</v>
@@ -5712,7 +5713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -5731,7 +5732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -5751,7 +5752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <f t="shared" si="11"/>
         <v>33</v>
@@ -5771,9 +5772,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
-        <f t="shared" ref="A261:A313" si="15">IF(MOD(ROW(A260)-1,8)=0,A260+1,A260)</f>
+        <f t="shared" ref="A261:A324" si="15">IF(MOD(ROW(A260)-1,8)=0,A260+1,A260)</f>
         <v>33</v>
       </c>
       <c r="B261" s="6">
@@ -5791,7 +5792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5811,7 +5812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5831,7 +5832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5851,7 +5852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <f t="shared" si="15"/>
         <v>33</v>
@@ -5871,7 +5872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5891,7 +5892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5911,7 +5912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5931,7 +5932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5951,7 +5952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5971,7 +5972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -5991,7 +5992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -6011,7 +6012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <f t="shared" si="15"/>
         <v>34</v>
@@ -6031,7 +6032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6051,7 +6052,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6071,7 +6072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6091,7 +6092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6111,7 +6112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6131,7 +6132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6151,7 +6152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6171,7 +6172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <f t="shared" si="15"/>
         <v>35</v>
@@ -6191,7 +6192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6211,7 +6212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6231,7 +6232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6251,7 +6252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6271,7 +6272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6291,7 +6292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6311,7 +6312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6331,7 +6332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <f t="shared" si="15"/>
         <v>36</v>
@@ -6351,7 +6352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6370,13 +6371,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="B291" s="6">
-        <f t="shared" ref="B290:B312" si="17">IF(A291="","",B290)</f>
+        <f t="shared" ref="B291:B312" si="17">IF(A291="","",B290)</f>
         <v>43597</v>
       </c>
       <c r="C291" t="str">
@@ -6390,7 +6391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6410,7 +6411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6430,7 +6431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6450,7 +6451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6470,7 +6471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6490,7 +6491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <f t="shared" si="15"/>
         <v>37</v>
@@ -6510,7 +6511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6530,7 +6531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6550,7 +6551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6570,7 +6571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6590,7 +6591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6610,7 +6611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6630,7 +6631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6650,7 +6651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <f t="shared" si="15"/>
         <v>38</v>
@@ -6670,7 +6671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6690,7 +6691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6710,7 +6711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6730,7 +6731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6750,7 +6751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6770,7 +6771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6790,7 +6791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
@@ -6810,17 +6811,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="B313" s="6">
-        <f t="shared" ref="B313" si="18">IF(A313="","",B312)</f>
+        <f t="shared" ref="B313:B320" si="18">IF(A313="","",B312)</f>
         <v>43597</v>
       </c>
       <c r="C313" t="str">
-        <f t="shared" ref="C313" si="19">IF(A313="","",C305)</f>
+        <f t="shared" ref="C313:C336" si="19">IF(A313="","",C305)</f>
         <v>Tim</v>
       </c>
       <c r="D313" s="2">
@@ -6830,751 +6831,1262 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="1"/>
-      <c r="B314" s="6"/>
-    </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="1"/>
-      <c r="B315" s="6"/>
-    </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A316" s="1"/>
-      <c r="B316" s="6"/>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A317" s="1"/>
-      <c r="B317" s="6"/>
-    </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" s="1"/>
-      <c r="B318" s="6"/>
-    </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A319" s="1"/>
-      <c r="B319" s="6"/>
-    </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A320" s="1"/>
-      <c r="B320" s="6"/>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="1"/>
-      <c r="B321" s="6"/>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" s="1"/>
-      <c r="B322" s="6"/>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" s="1"/>
-      <c r="B323" s="6"/>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="1"/>
-      <c r="B324" s="6"/>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="1"/>
-      <c r="B325" s="6"/>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="1"/>
-      <c r="B326" s="6"/>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="1"/>
-      <c r="B327" s="6"/>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="1"/>
-      <c r="B328" s="6"/>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="1"/>
-      <c r="B329" s="6"/>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="1"/>
-      <c r="B330" s="6"/>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="1"/>
-      <c r="B331" s="6"/>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="1"/>
-      <c r="B332" s="6"/>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="1"/>
-      <c r="B333" s="6"/>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="1"/>
-      <c r="B334" s="6"/>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="1"/>
-      <c r="B335" s="6"/>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="1"/>
-      <c r="B336" s="6"/>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" s="1"/>
-      <c r="B337" s="6"/>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" s="1"/>
-      <c r="B338" s="6"/>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" s="1"/>
-      <c r="B339" s="6"/>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="1"/>
-      <c r="B340" s="6"/>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" s="1"/>
-      <c r="B341" s="6"/>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" s="1"/>
-      <c r="B342" s="6"/>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" s="1"/>
-      <c r="B343" s="6"/>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" s="1"/>
-      <c r="B344" s="6"/>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" s="1"/>
-      <c r="B345" s="6"/>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A314" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B314" s="5">
+        <v>43702</v>
+      </c>
+      <c r="C314" t="str">
+        <f t="shared" si="19"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D314" s="2">
+        <v>15</v>
+      </c>
+      <c r="E314" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A315" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B315" s="6">
+        <f t="shared" si="18"/>
+        <v>43702</v>
+      </c>
+      <c r="C315" t="str">
+        <f t="shared" si="19"/>
+        <v>Alex</v>
+      </c>
+      <c r="D315" s="2">
+        <v>15</v>
+      </c>
+      <c r="E315" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A316" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B316" s="6">
+        <f t="shared" si="18"/>
+        <v>43702</v>
+      </c>
+      <c r="C316" t="str">
+        <f t="shared" si="19"/>
+        <v>Evan</v>
+      </c>
+      <c r="D316" s="2">
+        <v>15</v>
+      </c>
+      <c r="E316" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A317" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B317" s="6">
+        <f t="shared" si="18"/>
+        <v>43702</v>
+      </c>
+      <c r="C317" t="str">
+        <f t="shared" si="19"/>
+        <v>Andy</v>
+      </c>
+      <c r="D317" s="2">
+        <v>7</v>
+      </c>
+      <c r="E317" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A318" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B318" s="6">
+        <f t="shared" si="18"/>
+        <v>43702</v>
+      </c>
+      <c r="C318" t="str">
+        <f t="shared" si="19"/>
+        <v>Phil</v>
+      </c>
+      <c r="D318" s="2">
+        <v>7</v>
+      </c>
+      <c r="E318" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A319" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B319" s="6">
+        <f t="shared" si="18"/>
+        <v>43702</v>
+      </c>
+      <c r="C319" t="str">
+        <f t="shared" si="19"/>
+        <v>Ben</v>
+      </c>
+      <c r="D319" s="2">
+        <v>7</v>
+      </c>
+      <c r="E319" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A320" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B320" s="6">
+        <f t="shared" si="18"/>
+        <v>43702</v>
+      </c>
+      <c r="C320" t="str">
+        <f t="shared" si="19"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D320" s="2">
+        <v>15</v>
+      </c>
+      <c r="E320" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A321" s="1">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="B321" s="6">
+        <f t="shared" ref="B321:B361" si="20">IF(A321="","",B320)</f>
+        <v>43702</v>
+      </c>
+      <c r="C321" t="str">
+        <f t="shared" ref="C321:C361" si="21">IF(A321="","",C313)</f>
+        <v>Tim</v>
+      </c>
+      <c r="D321" s="2">
+        <v>7</v>
+      </c>
+      <c r="E321" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A322" s="1">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="B322" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C322" t="str">
+        <f t="shared" si="21"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D322" s="2">
+        <v>12</v>
+      </c>
+      <c r="E322" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A323" s="1">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="B323" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C323" t="str">
+        <f t="shared" si="21"/>
+        <v>Alex</v>
+      </c>
+      <c r="D323" s="2">
+        <v>15</v>
+      </c>
+      <c r="E323" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A324" s="1">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="B324" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C324" t="str">
+        <f t="shared" si="21"/>
+        <v>Evan</v>
+      </c>
+      <c r="D324" s="2">
+        <v>12</v>
+      </c>
+      <c r="E324" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A325" s="1">
+        <f t="shared" ref="A325:A361" si="22">IF(MOD(ROW(A324)-1,8)=0,A324+1,A324)</f>
+        <v>41</v>
+      </c>
+      <c r="B325" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C325" t="str">
+        <f t="shared" si="21"/>
+        <v>Andy</v>
+      </c>
+      <c r="D325" s="2">
+        <v>12</v>
+      </c>
+      <c r="E325" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A326" s="1">
+        <f t="shared" si="22"/>
+        <v>41</v>
+      </c>
+      <c r="B326" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C326" t="str">
+        <f t="shared" si="21"/>
+        <v>Phil</v>
+      </c>
+      <c r="D326" s="2">
+        <v>15</v>
+      </c>
+      <c r="E326" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A327" s="1">
+        <f t="shared" si="22"/>
+        <v>41</v>
+      </c>
+      <c r="B327" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C327" t="str">
+        <f t="shared" si="21"/>
+        <v>Ben</v>
+      </c>
+      <c r="D327" s="2">
+        <v>12</v>
+      </c>
+      <c r="E327" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A328" s="1">
+        <f t="shared" si="22"/>
+        <v>41</v>
+      </c>
+      <c r="B328" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C328" t="str">
+        <f t="shared" si="21"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D328" s="2">
+        <v>15</v>
+      </c>
+      <c r="E328" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A329" s="1">
+        <f t="shared" si="22"/>
+        <v>41</v>
+      </c>
+      <c r="B329" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C329" t="str">
+        <f t="shared" si="21"/>
+        <v>Tim</v>
+      </c>
+      <c r="D329" s="2">
+        <v>15</v>
+      </c>
+      <c r="E329" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A330" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B330" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C330" t="str">
+        <f t="shared" si="21"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D330" s="2">
+        <v>8</v>
+      </c>
+      <c r="E330" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A331" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B331" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C331" t="str">
+        <f t="shared" si="21"/>
+        <v>Alex</v>
+      </c>
+      <c r="D331" s="2">
+        <v>15</v>
+      </c>
+      <c r="E331" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A332" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B332" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C332" t="str">
+        <f t="shared" si="21"/>
+        <v>Evan</v>
+      </c>
+      <c r="D332" s="2">
+        <v>8</v>
+      </c>
+      <c r="E332" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A333" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B333" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C333" t="str">
+        <f t="shared" si="21"/>
+        <v>Andy</v>
+      </c>
+      <c r="D333" s="2">
+        <v>8</v>
+      </c>
+      <c r="E333" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A334" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B334" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C334" t="str">
+        <f t="shared" si="21"/>
+        <v>Phil</v>
+      </c>
+      <c r="D334" s="2">
+        <v>15</v>
+      </c>
+      <c r="E334" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A335" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B335" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C335" t="str">
+        <f t="shared" si="21"/>
+        <v>Ben</v>
+      </c>
+      <c r="D335" s="2">
+        <v>8</v>
+      </c>
+      <c r="E335" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A336" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B336" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C336" t="str">
+        <f t="shared" si="21"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D336" s="2">
+        <v>15</v>
+      </c>
+      <c r="E336" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A337" s="1">
+        <f t="shared" si="22"/>
+        <v>42</v>
+      </c>
+      <c r="B337" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C337" t="str">
+        <f t="shared" si="21"/>
+        <v>Tim</v>
+      </c>
+      <c r="D337" s="2">
+        <v>15</v>
+      </c>
+      <c r="E337" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A338" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B338" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C338" t="str">
+        <f t="shared" si="21"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D338" s="2">
+        <v>15</v>
+      </c>
+      <c r="E338" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A339" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B339" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C339" t="str">
+        <f t="shared" si="21"/>
+        <v>Alex</v>
+      </c>
+      <c r="D339" s="2">
+        <v>9</v>
+      </c>
+      <c r="E339" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A340" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B340" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C340" t="str">
+        <f t="shared" si="21"/>
+        <v>Evan</v>
+      </c>
+      <c r="D340" s="2">
+        <v>15</v>
+      </c>
+      <c r="E340" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A341" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B341" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C341" t="str">
+        <f t="shared" si="21"/>
+        <v>Andy</v>
+      </c>
+      <c r="D341" s="2">
+        <v>15</v>
+      </c>
+      <c r="E341" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A342" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B342" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C342" t="str">
+        <f t="shared" si="21"/>
+        <v>Phil</v>
+      </c>
+      <c r="D342" s="2">
+        <v>9</v>
+      </c>
+      <c r="E342" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A343" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B343" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C343" t="str">
+        <f t="shared" si="21"/>
+        <v>Ben</v>
+      </c>
+      <c r="D343" s="2">
+        <v>15</v>
+      </c>
+      <c r="E343" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A344" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B344" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C344" t="str">
+        <f t="shared" si="21"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D344" s="2">
+        <v>9</v>
+      </c>
+      <c r="E344" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A345" s="1">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="B345" s="6">
+        <f t="shared" si="20"/>
+        <v>43702</v>
+      </c>
+      <c r="C345" t="str">
+        <f t="shared" si="21"/>
+        <v>Tim</v>
+      </c>
+      <c r="D345" s="2">
+        <v>9</v>
+      </c>
+      <c r="E345" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" s="1"/>
       <c r="B346" s="6"/>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" s="1"/>
       <c r="B347" s="6"/>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" s="1"/>
       <c r="B348" s="6"/>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" s="1"/>
       <c r="B349" s="6"/>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" s="1"/>
       <c r="B350" s="6"/>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" s="1"/>
       <c r="B351" s="6"/>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" s="1"/>
       <c r="B352" s="6"/>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" s="1"/>
       <c r="B353" s="6"/>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" s="1"/>
       <c r="B354" s="6"/>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" s="1"/>
       <c r="B355" s="6"/>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" s="1"/>
       <c r="B356" s="6"/>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" s="1"/>
       <c r="B357" s="6"/>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" s="1"/>
       <c r="B358" s="6"/>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" s="1"/>
       <c r="B359" s="6"/>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" s="1"/>
       <c r="B360" s="6"/>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" s="1"/>
       <c r="B361" s="6"/>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" s="1"/>
       <c r="B362" s="6"/>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" s="1"/>
       <c r="B363" s="6"/>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="1"/>
       <c r="B364" s="6"/>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" s="1"/>
       <c r="B365" s="6"/>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" s="1"/>
       <c r="B366" s="6"/>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" s="1"/>
       <c r="B367" s="6"/>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" s="1"/>
       <c r="B368" s="6"/>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" s="1"/>
       <c r="B369" s="6"/>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="1"/>
       <c r="B370" s="6"/>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" s="1"/>
       <c r="B371" s="6"/>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" s="1"/>
       <c r="B372" s="6"/>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" s="1"/>
       <c r="B373" s="6"/>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" s="1"/>
       <c r="B374" s="6"/>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" s="1"/>
       <c r="B375" s="6"/>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" s="1"/>
       <c r="B376" s="6"/>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" s="1"/>
       <c r="B377" s="6"/>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" s="1"/>
       <c r="B378" s="6"/>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" s="1"/>
       <c r="B379" s="6"/>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" s="1"/>
       <c r="B380" s="6"/>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" s="1"/>
       <c r="B381" s="6"/>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" s="1"/>
       <c r="B382" s="6"/>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" s="1"/>
       <c r="B383" s="6"/>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" s="1"/>
       <c r="B384" s="6"/>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" s="1"/>
       <c r="B385" s="6"/>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" s="1"/>
       <c r="B386" s="6"/>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" s="1"/>
       <c r="B387" s="6"/>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" s="1"/>
       <c r="B388" s="6"/>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" s="1"/>
       <c r="B389" s="6"/>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" s="1"/>
       <c r="B390" s="6"/>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" s="1"/>
       <c r="B391" s="6"/>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" s="1"/>
       <c r="B392" s="6"/>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" s="1"/>
       <c r="B393" s="6"/>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" s="1"/>
       <c r="B394" s="6"/>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" s="1"/>
       <c r="B395" s="6"/>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" s="1"/>
       <c r="B396" s="6"/>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" s="1"/>
       <c r="B397" s="6"/>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" s="1"/>
       <c r="B398" s="6"/>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" s="1"/>
       <c r="B399" s="6"/>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" s="1"/>
       <c r="B400" s="6"/>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" s="1"/>
       <c r="B401" s="6"/>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" s="1"/>
       <c r="B402" s="6"/>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A403" s="1"/>
       <c r="B403" s="6"/>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A404" s="1"/>
       <c r="B404" s="6"/>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A405" s="1"/>
       <c r="B405" s="6"/>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A406" s="1"/>
       <c r="B406" s="6"/>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" s="1"/>
       <c r="B407" s="6"/>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A408" s="1"/>
       <c r="B408" s="6"/>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" s="1"/>
       <c r="B409" s="6"/>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A410" s="1"/>
       <c r="B410" s="6"/>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A411" s="1"/>
       <c r="B411" s="6"/>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A412" s="1"/>
       <c r="B412" s="6"/>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A413" s="1"/>
       <c r="B413" s="6"/>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A414" s="1"/>
       <c r="B414" s="6"/>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" s="1"/>
       <c r="B415" s="6"/>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A416" s="1"/>
       <c r="B416" s="6"/>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A417" s="1"/>
       <c r="B417" s="6"/>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A418" s="1"/>
       <c r="B418" s="6"/>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A419" s="1"/>
       <c r="B419" s="6"/>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A420" s="1"/>
       <c r="B420" s="6"/>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A421" s="1"/>
       <c r="B421" s="6"/>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A422" s="1"/>
       <c r="B422" s="6"/>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A423" s="1"/>
       <c r="B423" s="6"/>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A424" s="1"/>
       <c r="B424" s="6"/>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A425" s="1"/>
       <c r="B425" s="6"/>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A426" s="1"/>
       <c r="B426" s="6"/>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A427" s="1"/>
       <c r="B427" s="6"/>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A428" s="1"/>
       <c r="B428" s="6"/>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A429" s="1"/>
       <c r="B429" s="6"/>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A430" s="1"/>
       <c r="B430" s="6"/>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A431" s="1"/>
       <c r="B431" s="6"/>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A432" s="1"/>
       <c r="B432" s="6"/>
     </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A433" s="1"/>
       <c r="B433" s="6"/>
     </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A434" s="1"/>
       <c r="B434" s="6"/>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A435" s="1"/>
       <c r="B435" s="6"/>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A436" s="1"/>
       <c r="B436" s="6"/>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A437" s="1"/>
       <c r="B437" s="6"/>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A438" s="1"/>
       <c r="B438" s="6"/>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A439" s="1"/>
       <c r="B439" s="6"/>
     </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A440" s="1"/>
       <c r="B440" s="6"/>
     </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A441" s="1"/>
       <c r="B441" s="6"/>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A442" s="1"/>
       <c r="B442" s="6"/>
     </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A443" s="1"/>
       <c r="B443" s="6"/>
     </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A444" s="1"/>
       <c r="B444" s="6"/>
     </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A445" s="1"/>
       <c r="B445" s="6"/>
     </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A446" s="1"/>
       <c r="B446" s="6"/>
     </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A447" s="1"/>
       <c r="B447" s="6"/>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A448" s="1"/>
       <c r="B448" s="6"/>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A449" s="1"/>
       <c r="B449" s="6"/>
     </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A450" s="1"/>
       <c r="B450" s="6"/>
     </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A451" s="1"/>
       <c r="B451" s="6"/>
     </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A452" s="1"/>
       <c r="B452" s="6"/>
     </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A453" s="1"/>
       <c r="B453" s="6"/>
     </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A454" s="1"/>
       <c r="B454" s="6"/>
     </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A455" s="1"/>
       <c r="B455" s="6"/>
     </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A456" s="1"/>
       <c r="B456" s="6"/>
     </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A457" s="1"/>
       <c r="B457" s="6"/>
     </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A458" s="1"/>
       <c r="B458" s="6"/>
     </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A459" s="1"/>
       <c r="B459" s="6"/>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A460" s="1"/>
       <c r="B460" s="6"/>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A461" s="1"/>
       <c r="B461" s="6"/>
     </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A462" s="1"/>
       <c r="B462" s="6"/>
     </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A463" s="1"/>
       <c r="B463" s="6"/>
     </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A464" s="1"/>
       <c r="B464" s="6"/>
     </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A465" s="1"/>
       <c r="B465" s="6"/>
     </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A466" s="1"/>
       <c r="B466" s="6"/>
     </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A467" s="1"/>
       <c r="B467" s="6"/>
     </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A468" s="1"/>
       <c r="B468" s="6"/>
     </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A469" s="1"/>
       <c r="B469" s="6"/>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A470" s="1"/>
       <c r="B470" s="6"/>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A471" s="1"/>
       <c r="B471" s="6"/>
     </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A472" s="1"/>
       <c r="B472" s="6"/>
     </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A473" s="1"/>
       <c r="B473" s="6"/>
     </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A474" s="1"/>
       <c r="B474" s="6"/>
     </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A475" s="1"/>
       <c r="B475" s="6"/>
     </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A476" s="1"/>
       <c r="B476" s="6"/>
     </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A477" s="1"/>
       <c r="B477" s="6"/>
     </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" s="1"/>
       <c r="B478" s="6"/>
     </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A479" s="1"/>
       <c r="B479" s="6"/>
     </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480" s="1"/>
       <c r="B480" s="6"/>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A481" s="1"/>
       <c r="B481" s="6"/>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A482" s="1"/>
       <c r="B482" s="6"/>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A483" s="1"/>
       <c r="B483" s="6"/>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A484" s="1"/>
       <c r="B484" s="6"/>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A485" s="1"/>
       <c r="B485" s="6"/>
     </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A486" s="1"/>
       <c r="B486" s="6"/>
     </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A487" s="1"/>
       <c r="B487" s="6"/>
     </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A488" s="1"/>
       <c r="B488" s="6"/>
     </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A489" s="1"/>
       <c r="B489" s="6"/>
     </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A490" s="1"/>
       <c r="B490" s="6"/>
     </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A491" s="1"/>
       <c r="B491" s="6"/>
     </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A492" s="1"/>
       <c r="B492" s="6"/>
     </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A493" s="1"/>
       <c r="B493" s="6"/>
     </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A494" s="1"/>
       <c r="B494" s="6"/>
     </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495" s="1"/>
       <c r="B495" s="6"/>
     </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A496" s="1"/>
       <c r="B496" s="6"/>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497" s="1"/>
       <c r="B497" s="6"/>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A498" s="1"/>
       <c r="B498" s="6"/>
     </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A499" s="1"/>
       <c r="B499" s="6"/>
     </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A500" s="1"/>
       <c r="B500" s="6"/>
     </row>
@@ -7585,27 +8097,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -7667,7 +8179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>2019</v>
       </c>
@@ -7736,7 +8248,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <f t="shared" ref="A3:A9" si="0">A2</f>
         <v>2019</v>
@@ -7806,7 +8318,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7874,7 +8386,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7944,7 +8456,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8014,7 +8526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8084,7 +8596,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8154,7 +8666,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <f t="shared" si="0"/>
         <v>2019</v>

</xml_diff>

<commit_message>
Updated with Feb 8th 2020 data
</commit_message>
<xml_diff>
--- a/Basketball Stats.xlsx
+++ b/Basketball Stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\Desktop\Basketball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6D0C7-3B45-41F2-9588-8F6E3B5BA744}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7433AE-5C81-4A88-AB85-E134A04B5981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="H352" sqref="H352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6821,7 +6821,7 @@
         <v>43597</v>
       </c>
       <c r="C313" t="str">
-        <f t="shared" ref="C313:C336" si="19">IF(A313="","",C305)</f>
+        <f t="shared" ref="C313:C320" si="19">IF(A313="","",C305)</f>
         <v>Tim</v>
       </c>
       <c r="D313" s="2">
@@ -6976,11 +6976,11 @@
         <v>40</v>
       </c>
       <c r="B321" s="6">
-        <f t="shared" ref="B321:B361" si="20">IF(A321="","",B320)</f>
+        <f t="shared" ref="B321:B345" si="20">IF(A321="","",B320)</f>
         <v>43702</v>
       </c>
       <c r="C321" t="str">
-        <f t="shared" ref="C321:C361" si="21">IF(A321="","",C313)</f>
+        <f t="shared" ref="C321:C345" si="21">IF(A321="","",C313)</f>
         <v>Tim</v>
       </c>
       <c r="D321" s="2">
@@ -7052,7 +7052,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
-        <f t="shared" ref="A325:A361" si="22">IF(MOD(ROW(A324)-1,8)=0,A324+1,A324)</f>
+        <f t="shared" ref="A325:A388" si="22">IF(MOD(ROW(A324)-1,8)=0,A324+1,A324)</f>
         <v>41</v>
       </c>
       <c r="B325" s="6">
@@ -7471,158 +7471,542 @@
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A346" s="1"/>
-      <c r="B346" s="6"/>
+      <c r="A346" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B346" s="6">
+        <f t="shared" ref="B346:B389" si="23">IF(A346="","",B345)</f>
+        <v>43702</v>
+      </c>
+      <c r="C346" t="str">
+        <f t="shared" ref="C346:C389" si="24">IF(A346="","",C338)</f>
+        <v>RoBert</v>
+      </c>
+      <c r="D346" s="2">
+        <v>15</v>
+      </c>
+      <c r="E346" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A347" s="1"/>
-      <c r="B347" s="6"/>
+      <c r="A347" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B347" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C347" t="str">
+        <f t="shared" si="24"/>
+        <v>Alex</v>
+      </c>
+      <c r="D347" s="2">
+        <v>15</v>
+      </c>
+      <c r="E347" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A348" s="1"/>
-      <c r="B348" s="6"/>
+      <c r="A348" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B348" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C348" t="str">
+        <f t="shared" si="24"/>
+        <v>Evan</v>
+      </c>
+      <c r="D348" s="2">
+        <v>15</v>
+      </c>
+      <c r="E348" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A349" s="1"/>
-      <c r="B349" s="6"/>
+      <c r="A349" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B349" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C349" t="str">
+        <f t="shared" si="24"/>
+        <v>Andy</v>
+      </c>
+      <c r="D349" s="2">
+        <v>11</v>
+      </c>
+      <c r="E349" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A350" s="1"/>
-      <c r="B350" s="6"/>
+      <c r="A350" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B350" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C350" t="str">
+        <f t="shared" si="24"/>
+        <v>Phil</v>
+      </c>
+      <c r="D350" s="2">
+        <v>11</v>
+      </c>
+      <c r="E350" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A351" s="1"/>
-      <c r="B351" s="6"/>
+      <c r="A351" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B351" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C351" t="str">
+        <f t="shared" si="24"/>
+        <v>Ben</v>
+      </c>
+      <c r="D351" s="2">
+        <v>11</v>
+      </c>
+      <c r="E351" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A352" s="1"/>
-      <c r="B352" s="6"/>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A353" s="1"/>
-      <c r="B353" s="6"/>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A354" s="1"/>
-      <c r="B354" s="6"/>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A355" s="1"/>
-      <c r="B355" s="6"/>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A356" s="1"/>
-      <c r="B356" s="6"/>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A357" s="1"/>
-      <c r="B357" s="6"/>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A358" s="1"/>
-      <c r="B358" s="6"/>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A359" s="1"/>
-      <c r="B359" s="6"/>
-    </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A360" s="1"/>
-      <c r="B360" s="6"/>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A361" s="1"/>
-      <c r="B361" s="6"/>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A362" s="1"/>
-      <c r="B362" s="6"/>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A363" s="1"/>
-      <c r="B363" s="6"/>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A364" s="1"/>
-      <c r="B364" s="6"/>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A365" s="1"/>
-      <c r="B365" s="6"/>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A366" s="1"/>
-      <c r="B366" s="6"/>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A367" s="1"/>
-      <c r="B367" s="6"/>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A368" s="1"/>
-      <c r="B368" s="6"/>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A369" s="1"/>
-      <c r="B369" s="6"/>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A352" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B352" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C352" t="str">
+        <f t="shared" si="24"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D352" s="2">
+        <v>15</v>
+      </c>
+      <c r="E352" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A353" s="1">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="B353" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C353" t="str">
+        <f t="shared" si="24"/>
+        <v>Tim</v>
+      </c>
+      <c r="D353" s="2">
+        <v>11</v>
+      </c>
+      <c r="E353" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A354" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B354" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C354" t="str">
+        <f t="shared" si="24"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D354" s="2">
+        <v>7</v>
+      </c>
+      <c r="E354" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A355" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B355" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C355" t="str">
+        <f t="shared" si="24"/>
+        <v>Alex</v>
+      </c>
+      <c r="D355" s="2">
+        <v>15</v>
+      </c>
+      <c r="E355" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A356" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B356" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C356" t="str">
+        <f t="shared" si="24"/>
+        <v>Evan</v>
+      </c>
+      <c r="D356" s="2">
+        <v>15</v>
+      </c>
+      <c r="E356" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A357" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B357" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C357" t="str">
+        <f t="shared" si="24"/>
+        <v>Andy</v>
+      </c>
+      <c r="D357" s="2">
+        <v>7</v>
+      </c>
+      <c r="E357" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A358" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B358" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C358" t="str">
+        <f t="shared" si="24"/>
+        <v>Phil</v>
+      </c>
+      <c r="D358" s="2">
+        <v>7</v>
+      </c>
+      <c r="E358" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A359" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B359" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C359" t="str">
+        <f t="shared" si="24"/>
+        <v>Ben</v>
+      </c>
+      <c r="D359" s="2">
+        <v>15</v>
+      </c>
+      <c r="E359" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A360" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B360" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C360" t="str">
+        <f t="shared" si="24"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D360" s="2">
+        <v>7</v>
+      </c>
+      <c r="E360" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A361" s="1">
+        <f t="shared" si="22"/>
+        <v>45</v>
+      </c>
+      <c r="B361" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C361" t="str">
+        <f t="shared" si="24"/>
+        <v>Tim</v>
+      </c>
+      <c r="D361" s="2">
+        <v>15</v>
+      </c>
+      <c r="E361" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A362" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B362" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C362" t="str">
+        <f t="shared" si="24"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D362" s="2">
+        <v>20</v>
+      </c>
+      <c r="E362" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A363" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B363" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C363" t="str">
+        <f t="shared" si="24"/>
+        <v>Alex</v>
+      </c>
+      <c r="D363" s="2">
+        <v>20</v>
+      </c>
+      <c r="E363" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A364" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B364" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C364" t="str">
+        <f t="shared" si="24"/>
+        <v>Evan</v>
+      </c>
+      <c r="D364" s="2">
+        <v>20</v>
+      </c>
+      <c r="E364" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A365" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B365" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C365" t="str">
+        <f t="shared" si="24"/>
+        <v>Andy</v>
+      </c>
+      <c r="D365" s="2">
+        <v>20</v>
+      </c>
+      <c r="E365" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A366" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B366" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C366" t="str">
+        <f t="shared" si="24"/>
+        <v>Phil</v>
+      </c>
+      <c r="D366" s="2">
+        <v>20</v>
+      </c>
+      <c r="E366" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A367" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B367" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C367" t="str">
+        <f t="shared" si="24"/>
+        <v>Ben</v>
+      </c>
+      <c r="D367" s="2">
+        <v>20</v>
+      </c>
+      <c r="E367" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A368" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B368" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C368" t="str">
+        <f t="shared" si="24"/>
+        <v>Jeff</v>
+      </c>
+      <c r="D368" s="2">
+        <v>20</v>
+      </c>
+      <c r="E368" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A369" s="1">
+        <f t="shared" si="22"/>
+        <v>46</v>
+      </c>
+      <c r="B369" s="6">
+        <f t="shared" si="23"/>
+        <v>43702</v>
+      </c>
+      <c r="C369" t="str">
+        <f t="shared" si="24"/>
+        <v>Tim</v>
+      </c>
+      <c r="D369" s="2">
+        <v>20</v>
+      </c>
+      <c r="E369" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" s="1"/>
       <c r="B370" s="6"/>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" s="1"/>
       <c r="B371" s="6"/>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" s="1"/>
       <c r="B372" s="6"/>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" s="1"/>
       <c r="B373" s="6"/>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" s="1"/>
       <c r="B374" s="6"/>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" s="1"/>
       <c r="B375" s="6"/>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" s="1"/>
       <c r="B376" s="6"/>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" s="1"/>
       <c r="B377" s="6"/>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" s="1"/>
       <c r="B378" s="6"/>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" s="1"/>
       <c r="B379" s="6"/>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" s="1"/>
       <c r="B380" s="6"/>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" s="1"/>
       <c r="B381" s="6"/>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" s="1"/>
       <c r="B382" s="6"/>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" s="1"/>
       <c r="B383" s="6"/>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" s="1"/>
       <c r="B384" s="6"/>
     </row>

</xml_diff>

<commit_message>
Fixed the date (wasn't updated)
</commit_message>
<xml_diff>
--- a/Basketball Stats.xlsx
+++ b/Basketball Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\Desktop\Basketball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7433AE-5C81-4A88-AB85-E134A04B5981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7240FD0-E1CE-454C-9FC8-2D09BFE2A7A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -581,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A345" workbookViewId="0">
-      <selection activeCell="H352" sqref="H352"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="B347" sqref="B347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7052,7 +7054,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
-        <f t="shared" ref="A325:A388" si="22">IF(MOD(ROW(A324)-1,8)=0,A324+1,A324)</f>
+        <f t="shared" ref="A325:A369" si="22">IF(MOD(ROW(A324)-1,8)=0,A324+1,A324)</f>
         <v>41</v>
       </c>
       <c r="B325" s="6">
@@ -7475,12 +7477,11 @@
         <f t="shared" si="22"/>
         <v>44</v>
       </c>
-      <c r="B346" s="6">
-        <f t="shared" ref="B346:B389" si="23">IF(A346="","",B345)</f>
-        <v>43702</v>
+      <c r="B346" s="5">
+        <v>43869</v>
       </c>
       <c r="C346" t="str">
-        <f t="shared" ref="C346:C389" si="24">IF(A346="","",C338)</f>
+        <f t="shared" ref="C346:C369" si="23">IF(A346="","",C338)</f>
         <v>RoBert</v>
       </c>
       <c r="D346" s="2">
@@ -7496,11 +7497,11 @@
         <v>44</v>
       </c>
       <c r="B347" s="6">
+        <f t="shared" ref="B346:B369" si="24">IF(A347="","",B346)</f>
+        <v>43869</v>
+      </c>
+      <c r="C347" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C347" t="str">
-        <f t="shared" si="24"/>
         <v>Alex</v>
       </c>
       <c r="D347" s="2">
@@ -7516,11 +7517,11 @@
         <v>44</v>
       </c>
       <c r="B348" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C348" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C348" t="str">
-        <f t="shared" si="24"/>
         <v>Evan</v>
       </c>
       <c r="D348" s="2">
@@ -7536,11 +7537,11 @@
         <v>44</v>
       </c>
       <c r="B349" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C349" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C349" t="str">
-        <f t="shared" si="24"/>
         <v>Andy</v>
       </c>
       <c r="D349" s="2">
@@ -7556,11 +7557,11 @@
         <v>44</v>
       </c>
       <c r="B350" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C350" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C350" t="str">
-        <f t="shared" si="24"/>
         <v>Phil</v>
       </c>
       <c r="D350" s="2">
@@ -7576,11 +7577,11 @@
         <v>44</v>
       </c>
       <c r="B351" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C351" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C351" t="str">
-        <f t="shared" si="24"/>
         <v>Ben</v>
       </c>
       <c r="D351" s="2">
@@ -7596,11 +7597,11 @@
         <v>44</v>
       </c>
       <c r="B352" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C352" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C352" t="str">
-        <f t="shared" si="24"/>
         <v>Jeff</v>
       </c>
       <c r="D352" s="2">
@@ -7616,11 +7617,11 @@
         <v>44</v>
       </c>
       <c r="B353" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C353" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C353" t="str">
-        <f t="shared" si="24"/>
         <v>Tim</v>
       </c>
       <c r="D353" s="2">
@@ -7636,11 +7637,11 @@
         <v>45</v>
       </c>
       <c r="B354" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C354" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C354" t="str">
-        <f t="shared" si="24"/>
         <v>RoBert</v>
       </c>
       <c r="D354" s="2">
@@ -7656,11 +7657,11 @@
         <v>45</v>
       </c>
       <c r="B355" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C355" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C355" t="str">
-        <f t="shared" si="24"/>
         <v>Alex</v>
       </c>
       <c r="D355" s="2">
@@ -7676,11 +7677,11 @@
         <v>45</v>
       </c>
       <c r="B356" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C356" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C356" t="str">
-        <f t="shared" si="24"/>
         <v>Evan</v>
       </c>
       <c r="D356" s="2">
@@ -7696,11 +7697,11 @@
         <v>45</v>
       </c>
       <c r="B357" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C357" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C357" t="str">
-        <f t="shared" si="24"/>
         <v>Andy</v>
       </c>
       <c r="D357" s="2">
@@ -7716,11 +7717,11 @@
         <v>45</v>
       </c>
       <c r="B358" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C358" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C358" t="str">
-        <f t="shared" si="24"/>
         <v>Phil</v>
       </c>
       <c r="D358" s="2">
@@ -7736,11 +7737,11 @@
         <v>45</v>
       </c>
       <c r="B359" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C359" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C359" t="str">
-        <f t="shared" si="24"/>
         <v>Ben</v>
       </c>
       <c r="D359" s="2">
@@ -7756,11 +7757,11 @@
         <v>45</v>
       </c>
       <c r="B360" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C360" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C360" t="str">
-        <f t="shared" si="24"/>
         <v>Jeff</v>
       </c>
       <c r="D360" s="2">
@@ -7776,11 +7777,11 @@
         <v>45</v>
       </c>
       <c r="B361" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C361" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C361" t="str">
-        <f t="shared" si="24"/>
         <v>Tim</v>
       </c>
       <c r="D361" s="2">
@@ -7796,11 +7797,11 @@
         <v>46</v>
       </c>
       <c r="B362" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C362" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C362" t="str">
-        <f t="shared" si="24"/>
         <v>RoBert</v>
       </c>
       <c r="D362" s="2">
@@ -7816,11 +7817,11 @@
         <v>46</v>
       </c>
       <c r="B363" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C363" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C363" t="str">
-        <f t="shared" si="24"/>
         <v>Alex</v>
       </c>
       <c r="D363" s="2">
@@ -7836,11 +7837,11 @@
         <v>46</v>
       </c>
       <c r="B364" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C364" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C364" t="str">
-        <f t="shared" si="24"/>
         <v>Evan</v>
       </c>
       <c r="D364" s="2">
@@ -7856,11 +7857,11 @@
         <v>46</v>
       </c>
       <c r="B365" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C365" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C365" t="str">
-        <f t="shared" si="24"/>
         <v>Andy</v>
       </c>
       <c r="D365" s="2">
@@ -7876,11 +7877,11 @@
         <v>46</v>
       </c>
       <c r="B366" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C366" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C366" t="str">
-        <f t="shared" si="24"/>
         <v>Phil</v>
       </c>
       <c r="D366" s="2">
@@ -7896,11 +7897,11 @@
         <v>46</v>
       </c>
       <c r="B367" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C367" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C367" t="str">
-        <f t="shared" si="24"/>
         <v>Ben</v>
       </c>
       <c r="D367" s="2">
@@ -7916,11 +7917,11 @@
         <v>46</v>
       </c>
       <c r="B368" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C368" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C368" t="str">
-        <f t="shared" si="24"/>
         <v>Jeff</v>
       </c>
       <c r="D368" s="2">
@@ -7936,11 +7937,11 @@
         <v>46</v>
       </c>
       <c r="B369" s="6">
+        <f t="shared" si="24"/>
+        <v>43869</v>
+      </c>
+      <c r="C369" t="str">
         <f t="shared" si="23"/>
-        <v>43702</v>
-      </c>
-      <c r="C369" t="str">
-        <f t="shared" si="24"/>
         <v>Tim</v>
       </c>
       <c r="D369" s="2">

</xml_diff>